<commit_message>
change menu and add items
</commit_message>
<xml_diff>
--- a/Excel_files/Hotels.xlsx
+++ b/Excel_files/Hotels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SIVAGAMI\eclipse-workspace\orderapp\Excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F787F84-41A1-43CA-B7CC-142AEA56A9F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E726EB2-3883-4FC7-823A-68E4199DBEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{3EF13A9E-E041-4EA5-A92C-9E892B3AEB68}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{3EF13A9E-E041-4EA5-A92C-9E892B3AEB68}"/>
   </bookViews>
   <sheets>
     <sheet name="Thalapakatti" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Copper Kitchen" sheetId="3" r:id="rId3"/>
     <sheet name="A2B" sheetId="4" r:id="rId4"/>
     <sheet name="Gupta bhavan" sheetId="6" r:id="rId5"/>
+    <sheet name="Sunset" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
   <si>
     <t>Vada</t>
   </si>
@@ -158,13 +159,40 @@
   </si>
   <si>
     <t>Laddu</t>
+  </si>
+  <si>
+    <t>Falooda</t>
+  </si>
+  <si>
+    <t>Tandoori</t>
+  </si>
+  <si>
+    <t>Grill Chicken</t>
+  </si>
+  <si>
+    <t>Chicken Drumstick</t>
+  </si>
+  <si>
+    <t>Chicken Fry</t>
+  </si>
+  <si>
+    <t>Cream Pasta</t>
+  </si>
+  <si>
+    <t>Cheese Maggi</t>
+  </si>
+  <si>
+    <t>Paneer Friedrice</t>
+  </si>
+  <si>
+    <t>Chicken Friedrice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +212,12 @@
       <sz val="10"/>
       <color rgb="FF0D0D0D"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -213,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -223,6 +257,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,10 +642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F5B75E-DB48-45C2-ADF8-83510CFE04DA}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,7 +666,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.35">
@@ -639,7 +674,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="3">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.35">
@@ -680,6 +715,46 @@
       </c>
       <c r="B8" s="3">
         <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -803,7 +878,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B253226-D847-4527-A8B4-D6180B286C07}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H14" activeCellId="1" sqref="A3 H14"/>
@@ -910,6 +985,14 @@
         <v>115</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -919,7 +1002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -963,4 +1046,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>180</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>